<commit_message>
RNAscope: fix redundancy/typos in some reference expression matrices
</commit_message>
<xml_diff>
--- a/rnascope/raw_data/Star_expected_expression_revisionMNT.xlsx
+++ b/rnascope/raw_data/Star_expected_expression_revisionMNT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10711"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattntran/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD029C0-A740-5C4D-9E68-00A57C46B866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F6C2B5-7EF5-E14C-99D9-7DB18CE42EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="19100" windowHeight="8780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9120" yWindow="4500" windowWidth="19100" windowHeight="8780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
     <t>D2_C</t>
   </si>
   <si>
-    <t>D2_A/B/C</t>
+    <t>D2_A/B/D</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>